<commit_message>
Tar med info tab i import-exelark
</commit_message>
<xml_diff>
--- a/src/main/resources/substituttlister/V1_personloftere.xlsx
+++ b/src/main/resources/substituttlister/V1_personloftere.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasmund/dev/hm-grunndata-alternativprodukter/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasmund/dev/hm-grunndata-alternativprodukter/src/main/resources/substituttlister/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80D0C353-05AD-5940-B84A-CD9B223D1381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E34E084-B4D4-5342-BB53-A4C8F0B413EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16780" xr2:uid="{8997ABA3-265C-4565-AD00-094E7F16CC3A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16460" xr2:uid="{8997ABA3-265C-4565-AD00-094E7F16CC3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark2" sheetId="2" r:id="rId1"/>
+    <sheet name="Ark1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -813,10 +814,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B4AD1C-A47C-AB4A-AD3E-147D156EDDD0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815AA82E-56E2-4B74-827D-F4710CA2D241}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>

</xml_diff>